<commit_message>
Code includes a new test case about the new dashboard
</commit_message>
<xml_diff>
--- a/resources/DataSheet.xlsx
+++ b/resources/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16065" windowHeight="3705"/>
+    <workbookView windowWidth="16545" windowHeight="3705" firstSheet="15" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Values To Enter in JavaScript" sheetId="14" r:id="rId15"/>
     <sheet name="Reports Verification" sheetId="16" r:id="rId16"/>
     <sheet name="Quick Edits" sheetId="17" r:id="rId17"/>
+    <sheet name="New Dashboard" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C3"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
   <si>
     <t>User Type</t>
   </si>
@@ -75,16 +76,16 @@
     <t>Comp Admin Created</t>
   </si>
   <si>
-    <t>savita+637166@infrrd.ai</t>
-  </si>
-  <si>
-    <t>Company1637166</t>
+    <t>savita+256352@infrrd.ai</t>
+  </si>
+  <si>
+    <t>Company1256352</t>
   </si>
   <si>
     <t>Agent Created</t>
   </si>
   <si>
-    <t>savita+6371661@infrrd.ai</t>
+    <t>savita+2563521@infrrd.ai</t>
   </si>
   <si>
     <t>infrrd@socialsurvey.com</t>
@@ -132,6 +133,9 @@
     <t>Quick Edits</t>
   </si>
   <si>
+    <t>New Dashboard</t>
+  </si>
+  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -315,16 +319,7 @@
     <t>Chicago Office</t>
   </si>
   <si>
-    <t>Derek Jeter</t>
-  </si>
-  <si>
-    <t>Summit Funding, Inc.</t>
-  </si>
-  <si>
-    <t>Reed Region</t>
-  </si>
-  <si>
-    <t>Baton Rouge, LA</t>
+    <t>Dwayne Wade</t>
   </si>
   <si>
     <t>SavitaStaging Widgets</t>
@@ -498,19 +493,75 @@
     <t>Test Disclaimer</t>
   </si>
   <si>
-    <t>savita+392786@infrrd.ai</t>
-  </si>
-  <si>
-    <t>Company1392786</t>
-  </si>
-  <si>
-    <t>savita+686958@infrrd.ai</t>
-  </si>
-  <si>
-    <t>Company1686958</t>
-  </si>
-  <si>
-    <t>savita+6869581@infrrd.ai</t>
+    <t>Processed Count</t>
+  </si>
+  <si>
+    <t>Completed Count</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Social Posts</t>
+  </si>
+  <si>
+    <t>Zillow Reviews</t>
+  </si>
+  <si>
+    <t>Third Party Reviews</t>
+  </si>
+  <si>
+    <t>Google Reviews</t>
+  </si>
+  <si>
+    <t>Facebook Reviews</t>
+  </si>
+  <si>
+    <t>Unprocessed</t>
+  </si>
+  <si>
+    <t>Unassigned</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Corrupted</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Unsubscribed</t>
+  </si>
+  <si>
+    <t>select count(*) as Count from ss_report_demo.survey_details where AGENT_ID in 
+(select USER_ID from ss_report_demo.users where COMPANY_ID=909 and STATUS in (1,2)) 
+and STAGE =-1 and SOURCE not in ("Zillow","3rd Party Review");</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_pre_initiation where COMPANY_ID=909 and status in (0,1,2);</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_details where COMPANY_ID=909 and SOURCE like 'Zillow';</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_details where COMPANY_ID=909 and SOURCE like '3rd Party Review';</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_details where COMPANY_ID=909 and SOURCE like 'google';</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_details where COMPANY_ID=909 and SOURCE like 'facebook';</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_pre_initiation where COMPANY_ID=909 and status=10;</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_pre_initiation where COMPANY_ID=909 and status=5;</t>
+  </si>
+  <si>
+    <t>select count(*) from ss_report_demo.survey_pre_initiation where COMPANY_ID=909 and status=8;</t>
   </si>
 </sst>
 </file>
@@ -519,8 +570,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="181" formatCode="[$-14009]dd/mm/yyyy;@"/>
@@ -577,32 +628,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -614,9 +650,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -630,16 +665,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -659,28 +694,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -691,7 +704,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -703,6 +723,37 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -710,6 +761,78 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -719,13 +842,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,13 +866,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,67 +890,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,42 +932,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -875,25 +944,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,17 +982,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,26 +1027,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -996,26 +1064,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,154 +1075,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1207,14 +1270,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1238,6 +1298,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1570,158 +1633,158 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.8571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.8571428571429" collapsed="true"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="22.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="28.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:8">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="G2" s="23" t="s">
+      <c r="D2" s="16"/>
+      <c r="G2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" ht="30" spans="1:8">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>158</v>
+      <c r="D4" s="16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:9">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="G5" s="25" t="s">
+      <c r="D5" s="16"/>
+      <c r="G5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" ht="60" spans="1:6">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" ht="135" spans="1:7">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G9" t="s">
@@ -1729,26 +1792,40 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" ht="30" spans="1:4">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1763,6 +1840,7 @@
     <hyperlink ref="I5" r:id="rId3" display="stagingtest@socialsurvey.com"/>
     <hyperlink ref="C3" r:id="rId4" display="Kamala@19" tooltip="mailto:Kamala@19"/>
     <hyperlink ref="B3" r:id="rId5" display="savita@infrrd.ai"/>
+    <hyperlink ref="C12" r:id="rId2" display="Test@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1780,23 +1858,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.1428571428571" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.1428571428571" collapsed="true"/>
+    <col min="1" max="1" width="30.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.1428571428571" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1820,64 +1898,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.4285714285714" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.7142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.8571428571429" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="30.5714285714286" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.1428571428571" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="25.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.4285714285714" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="13">
+      <c r="F2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="17">
         <v>6</v>
       </c>
     </row>
@@ -1898,23 +1976,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.5714285714286" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.5714285714286" collapsed="true"/>
+    <col min="1" max="1" width="27.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.5714285714286" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="15">
+      <c r="A2" s="18">
         <v>43101</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="19">
         <v>43465</v>
       </c>
     </row>
@@ -1930,43 +2008,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.8571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.8571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="1" max="1" width="21.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="21.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="22.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="17" t="s">
         <v>94</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1978,44 +2056,50 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="21" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="16384" customWidth="true" style="11" width="21.0" collapsed="true"/>
+    <col min="1" max="16384" width="21" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="D1" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:4">
+      <c r="A2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>98</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2034,127 +2118,127 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="5" width="21.1428571428571" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="24.4285714285714" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.4285714285714" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="24.1428571428571" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="5" width="25.2857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="5" width="81.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="93.8571428571429" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="5" width="13.4285714285714" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="5" width="22.1428571428571" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="5" width="7.14285714285714" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="5" width="24.7142857142857" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="5" width="27.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="5" width="25.7142857142857" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="5" width="27.5714285714286" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="5" width="24.7142857142857" collapsed="true"/>
-    <col min="17" max="16384" style="5" width="9.14285714285714" collapsed="true"/>
+    <col min="1" max="2" width="21.1428571428571" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.4285714285714" style="9" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.4285714285714" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.1428571428571" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.2857142857143" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="81" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="93.8571428571429" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.4285714285714" style="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.1428571428571" style="9" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.14285714285714" style="9" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.7142857142857" style="9" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27" style="9" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.7142857142857" style="9" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.5714285714286" style="9" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.7142857142857" style="9" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="9.14285714285714" style="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12">
+        <v>200</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="H2" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8">
-        <v>5</v>
-      </c>
-      <c r="F2" s="8">
-        <v>200</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="M2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2177,45 +2261,45 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.8571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.8571428571429" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="25.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="12.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2230,196 +2314,196 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="T1" sqref="T1:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.4285714285714" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.7142857142857" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.4285714285714" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.2857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.8571428571429" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.4285714285714" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.1428571428571" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="10.1428571428571" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" width="9.71428571428571" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.8571428571429" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="6.14285714285714" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="14.4285714285714" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="6.57142857142857" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="14.7142857142857" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="19.4285714285714" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="26.7142857142857" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="15.5714285714286" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="25.2857142857143" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="17.8571428571429" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="17.4285714285714" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="12.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="25.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="15.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="14.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="16.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="10.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="16.4285714285714" customWidth="1"/>
+    <col min="9" max="9" width="11.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="10.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="14" width="9.71428571428571" customWidth="1"/>
+    <col min="15" max="15" width="13.8571428571429" customWidth="1"/>
+    <col min="16" max="16" width="6.14285714285714" customWidth="1"/>
+    <col min="17" max="17" width="14.4285714285714" customWidth="1"/>
+    <col min="18" max="18" width="6.57142857142857" customWidth="1"/>
+    <col min="19" max="19" width="14.7142857142857" customWidth="1"/>
+    <col min="20" max="20" width="19.4285714285714" customWidth="1"/>
+    <col min="21" max="21" width="26.7142857142857" customWidth="1"/>
+    <col min="22" max="22" width="15.5714285714286" customWidth="1"/>
+    <col min="23" max="23" width="25.2857142857143" customWidth="1"/>
+    <col min="24" max="24" width="17.8571428571429" customWidth="1"/>
+    <col min="25" max="25" width="17.4285714285714" customWidth="1"/>
+    <col min="26" max="26" width="12.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="Y1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="K2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="Q2" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="K2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="b">
+      <c r="R2" s="6">
+        <v>90001</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="W2" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="X2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" s="2">
-        <v>90001</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="W2" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="X2" s="2" t="b">
+      <c r="Y2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Y2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>123</v>
+      <c r="Z2" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2428,6 +2512,118 @@
     <hyperlink ref="T2" r:id="rId2" display="www.testweb.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1428571428571" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.8571428571429" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5714285714286" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1428571428571" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.71428571428571" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1428571428571" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" ht="210" spans="1:14">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2443,37 +2639,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.5714285714286" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.7142857142857" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.8571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.1428571428571" collapsed="true"/>
+    <col min="1" max="1" width="12.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1428571428571" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="D1" s="20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2499,30 +2695,30 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2538,77 +2734,77 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.2857142857143" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.1428571428571" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.57142857142857" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.14285714285714" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="8.85714285714286" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.7142857142857" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="16.2857142857143" customWidth="1"/>
+    <col min="2" max="3" width="10.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="8.57142857142857" customWidth="1"/>
+    <col min="5" max="5" width="6.14285714285714" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="8.85714285714286" customWidth="1"/>
+    <col min="8" max="8" width="16.7142857142857" customWidth="1"/>
+    <col min="9" max="9" width="14.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="20" t="s">
         <v>47</v>
       </c>
+      <c r="I1" s="20" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="A2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="18">
+      <c r="F2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="21">
         <v>10001</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="21" t="s">
         <v>53</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2628,64 +2824,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.8571428571429" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.1428571428571" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.8571428571429" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.14285714285714" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.28571428571429" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
+    <col min="2" max="3" width="10.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="13.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="6.14285714285714" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.28571428571429" customWidth="1"/>
+    <col min="8" max="8" width="16.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="A1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>55</v>
+      <c r="G1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="A2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="18">
+      <c r="F2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="21">
         <v>10001</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2709,78 +2905,78 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.1428571428571" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.8571428571429" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="6.14285714285714" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="9.28571428571429" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.4285714285714" collapsed="true"/>
+    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.85714285714286" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.14285714285714" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.28571428571429" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.4285714285714" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="D2" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="E2" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="F2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="18">
+      <c r="H2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="21">
         <v>10001</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2804,29 +3000,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.85714285714286" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="9.85714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7142857142857" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="A1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2848,29 +3044,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="11.2857142857143" collapsed="true"/>
+    <col min="1" max="3" width="11.2857142857143" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>67</v>
       </c>
+      <c r="C1" s="20" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="23" t="s">
         <v>67</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2890,35 +3086,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.5714285714286" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.2857142857143" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.8571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="11.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="A1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>69</v>
+      <c r="C1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SPS changes in new dashboard test case
</commit_message>
<xml_diff>
--- a/resources/DataSheet.xlsx
+++ b/resources/DataSheet.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="182">
   <si>
     <t>User Type</t>
   </si>
@@ -533,6 +533,15 @@
   </si>
   <si>
     <t>Unsubscribed</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Unpleasant</t>
   </si>
   <si>
     <t>select count(*) as Count from ss_report_demo.survey_details where AGENT_ID in 
@@ -562,6 +571,15 @@
   </si>
   <si>
     <t>select count(*) from ss_report_demo.survey_pre_initiation where COMPANY_ID=909 and status=8;</t>
+  </si>
+  <si>
+    <t>select count(*) from survey_details where COMPANY_ID=909 and SOURCE not in('Zillow' ,'3rd Party Review') and MOOD like 'Great';</t>
+  </si>
+  <si>
+    <t>select count(*) from survey_details where COMPANY_ID=909 and SOURCE not in('Zillow' ,'3rd Party Review') and MOOD like 'OK';</t>
+  </si>
+  <si>
+    <t>select count(*) from survey_details where COMPANY_ID=909 and SOURCE not in('Zillow' ,'3rd Party Review') and MOOD like 'Unpleasant';</t>
   </si>
 </sst>
 </file>
@@ -569,11 +587,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="24">
@@ -628,7 +646,47 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,32 +700,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -687,21 +721,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -711,14 +730,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,7 +752,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -747,11 +766,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -764,7 +782,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,7 +908,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,79 +920,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,67 +944,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -944,7 +956,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,6 +994,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -993,36 +1020,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,11 +1059,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1075,7 +1093,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1087,136 +1108,133 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1278,7 +1296,7 @@
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -2519,10 +2537,10 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2541,10 +2559,12 @@
     <col min="12" max="12" width="10.5714285714286" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.71428571428571" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.1428571428571" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.14285714285714" style="1"/>
+    <col min="15" max="16" width="9.14285714285714" style="1"/>
+    <col min="17" max="17" width="9" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" ht="30" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -2587,40 +2607,58 @@
       <c r="N1" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" ht="210" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" ht="300" spans="1:17">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
+      <c r="O2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>